<commit_message>
Until Part 2 Chapter 12
</commit_message>
<xml_diff>
--- a/P2C12/example.xlsx
+++ b/P2C12/example.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>Apples</t>
   </si>
@@ -40,15 +40,12 @@
   <si>
     <t>Strawberries</t>
   </si>
-  <si>
-    <t>check</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +58,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,7 +87,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -94,6 +98,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,15 +437,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" style="4" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -518,11 +524,6 @@
       </c>
       <c r="C7" s="3">
         <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H21" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>